<commit_message>
Fixed the original data and added output data. Added headings, graphs, and preliminary work on DML.
</commit_message>
<xml_diff>
--- a/data/env_waste_mun.xlsx
+++ b/data/env_waste_mun.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anna\research_module\RM-project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76C2BC7B-4889-47D2-BF77-D6DA32EDC7DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC77D912-F141-4F9A-AADC-D744B45AD95F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="633" uniqueCount="102">
   <si>
     <t>Municipal waste by waste management operations [env_wasmun$defaultview]</t>
   </si>
@@ -338,7 +338,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -378,6 +378,22 @@
       <u/>
       <sz val="9"/>
       <color indexed="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="204"/>
@@ -443,7 +459,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -489,6 +505,12 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -888,22 +910,22 @@
       <c r="A8" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
-      <c r="J8" s="18"/>
-      <c r="K8" s="18"/>
-      <c r="L8" s="18"/>
-      <c r="M8" s="18"/>
-      <c r="N8" s="18"/>
-      <c r="O8" s="18"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="20"/>
+      <c r="L8" s="20"/>
+      <c r="M8" s="20"/>
+      <c r="N8" s="20"/>
+      <c r="O8" s="20"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
@@ -1624,10 +1646,10 @@
   <dimension ref="A1:K42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C12" sqref="C12"/>
+      <selection pane="bottomRight" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.4" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1917,7 +1939,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="18" t="s">
         <v>49</v>
       </c>
       <c r="B9" s="9" t="s">
@@ -1926,8 +1948,8 @@
       <c r="C9" s="9">
         <v>562</v>
       </c>
-      <c r="D9" s="9" t="s">
-        <v>96</v>
+      <c r="D9" s="9">
+        <v>571</v>
       </c>
       <c r="E9" s="9">
         <v>580</v>
@@ -1944,11 +1966,11 @@
       <c r="I9" s="9">
         <v>637</v>
       </c>
-      <c r="J9" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="K9" s="9" t="s">
-        <v>96</v>
+      <c r="J9" s="9">
+        <v>625</v>
+      </c>
+      <c r="K9" s="9">
+        <v>622</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
@@ -2057,7 +2079,7 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="17" t="s">
         <v>53</v>
       </c>
       <c r="B13" s="9">
@@ -2652,7 +2674,7 @@
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A30" s="6" t="s">
+      <c r="A30" s="17" t="s">
         <v>70</v>
       </c>
       <c r="B30" s="8">

</xml_diff>

<commit_message>
Removed waste values calculated with the old methodology. Add a variable Group, correlation analysis, OLS regression, and DML IRM model.
</commit_message>
<xml_diff>
--- a/data/env_waste_mun.xlsx
+++ b/data/env_waste_mun.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anna\research_module\RM-project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC77D912-F141-4F9A-AADC-D744B45AD95F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EE1D7EB-1977-48C6-AE1A-6493E6C8DA58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="633" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="102">
   <si>
     <t>Municipal waste by waste management operations [env_wasmun$defaultview]</t>
   </si>
@@ -1646,10 +1646,10 @@
   <dimension ref="A1:K42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B18" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B24" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A9" sqref="A9"/>
+      <selection pane="bottomRight" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.4" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -3024,17 +3024,11 @@
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A41" s="1" t="s">
-        <v>97</v>
-      </c>
+      <c r="A41" s="1"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A42" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>98</v>
-      </c>
+      <c r="A42" s="1"/>
+      <c r="B42" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>